<commit_message>
Added image questions & answers
I'm so sorry kenneth LOL
</commit_message>
<xml_diff>
--- a/SAT_Tester_v2/data/testing/test_questions/SAT_Test_1.xlsx
+++ b/SAT_Tester_v2/data/testing/test_questions/SAT_Test_1.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pampperin\Documents\GitHub\SAT_Test_Engine\SAT_Tester_v2\resources\testing\test_questions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pampperin\Documents\GitHub\SAT_Test_Engine\SAT_Tester_v2\data\testing\test_questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15510" windowHeight="8145"/>
   </bookViews>
   <sheets>
-    <sheet name="Book1" sheetId="1" r:id="rId1"/>
+    <sheet name="SAT_Test_1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Kathy repairs phones at a rate of 108 per day</t>
   </si>
@@ -100,6 +100,27 @@
   </si>
   <si>
     <t>Question</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Which of the following graphs best shows a strong negative association between d and t?</t>
+  </si>
+  <si>
+    <t>QuestionImage</t>
+  </si>
+  <si>
+    <t>Answer Image</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
@@ -420,100 +441,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>